<commit_message>
add fake coffe data
</commit_message>
<xml_diff>
--- a/src/utils/coffee.xlsx
+++ b/src/utils/coffee.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="152">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -49,27 +49,582 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>拿铁</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RMB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>latte</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>latte</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>32RMB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5b56daaaebf8b363b6f8954f</t>
+    <t>小红莓金汤力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>杯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>imageUrl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>经典金汤力基础上加入蔓越莓，重新定义这款鸡尾酒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当跳跃的红色蔓越莓落入汤力水的怀抱，莓果的酸甜平衡了金酒的辛辣，还将汤力水的微苦修饰得恰到好处，和冰块一起带来刺激爽快的口感，没人能够拒绝。未成年请勿饮酒，酒后请勿驾驶。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>descriptionUrl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1530599314713.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>经典莫吉托</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>含酒精且含气，12oz，未成年人请勿饮酒，酒后请勿驾驶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>杯经典的青柠莫吉托永不过时。选用百加得白朗姆酒搭配青柠、薄荷、苏打水，清凉的薄荷散发出迷人气息，欲擒故纵的最佳范本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1529910576711.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1523957013951.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>仲夏莫吉托</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在经典莫吉托的基础上加入热情的菠萝，搭配活泼的青柠，仲夏的激情从此刻开始点燃，什么都别说了，跟上节奏，舞池的C位属于你</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>含酒精且含气，12oz，未成年人请勿饮酒，酒后请勿驾驶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1530599806317.jpeg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1529910601218.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1523957039434.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sort</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>长岛冰茶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>李诞同款，酒劲十足，未成年请勿饮酒，酒后请勿驾驶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在经典长岛冰茶基础上，将可乐升级为南非国宝茶路易波士，温和甘甜的低调外表下，加入多款百加得经典基酒，隐藏了令人刮目相看的后作力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1529910504894.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1527230326996.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>柚见佳人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红西柚风味鸡尾酒，未成年请勿饮酒，酒后请勿驾驶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红西柚风味结合百加得孟买蓝宝石金酒的植物芬芳，酸甜清新，层次丰富。顶部漂浮的慕斯奶沫让口感变得更加润滑，柔美粉红色让人好感度倍增</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1528969795096.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1528876843415.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天生的粉椰子水</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>泰国进口Nam Hom椰子水，天生粉色，好喝颜值高</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>未经高温处理的新鲜泰国Nam Hom嫩椰水，经过光照，部分椰子水会变成幸运的粉红色，天生高颜值。不含添加糖，健康无负担，不含咖啡因</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5b6277cb12d3ed723614ba09</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5b6277cb12d3ed723614ba08</t>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1521785265435.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/product/702/product_describe.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生气的粉椰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>带气泡的粉色椰子水，同时拥有清甜椰香与酷爽口感</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每一口都冒着少女心的粉色气泡，包裹着椰子的香气，从口腔狂奔到喉咙的清凉感，一扫炎夏的粘腻。不含添加糖，健康无负担，不含咖啡因</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1526548321042.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1526461796573.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>打气的麦芽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无酒精的“啤酒”，拥有醇正麦芽香，鼓足气，嘬一口冰爽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>十足的啤酒麦芽香，细腻丰富的泡沫，伴着激烈的夏日赛事，无酒精，却能让你更加沉醉。如果麦芽也是球迷，它一定会鼓足了劲加油「打气」</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1528446508988.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1528446510428.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>打气的玫瑰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无酒精的“啤酒”中透出玫瑰花香，鼓足气，嘬一口冰爽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在「打气的麦芽」中放入大朵优质可食用的“重瓣玫瑰”，甜甜的幸福感在心中绽放。进球的瞬间，心中乐出朵朵玫瑰花，就知道没白「打气」</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1528446580569.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1528446581578.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冷萃咖啡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>24小时低温萃取，独有坚果、可可和麦芽糖香气</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冷萃专用咖啡豆，甜度极佳、酸感轻柔舒适，具有强劲的厚实感和迷人的花果香气。Crema细腻丰厚，独有坚果、可可和麦芽糖的甜香气</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5b6277cb12d3ed723614ba0a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1526026192944.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1526035281497.jpeg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生气的冷萃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有气泡的冷萃，咖啡香气在气泡的鼓动下在舌尖炸开</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>24小时低温萃取的冷萃，甜度极佳、酸感轻柔舒适，有些许香橙风味。冷萃咖啡恰到好处的酸度混合热带水果柔和香气，在气泡的鼓动下在舌尖炸开</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1526458528866.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1526035301563.jpeg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰美式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>精确比例拼配6支阿拉比卡咖啡豆，与众不同的惊艳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前段体现出独特的乌梅酒香，同时带有黑醋栗般的尾韵与高甜度的口感。低温放大了咖啡豆的独特风味，口感扎实丰富且尾韵绵延细长</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/product/473/cafe_convert.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1519968003764.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5b6277cb12d3ed723614ba0a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5b6277cb12d3ed723614ba0a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰拿铁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>精选拼配阿拉比卡咖啡豆，配上优质牛奶，甜感十足</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>口感均衡细滑的浓缩咖啡，加入牛奶后展现出热带水果的香甜味，降至冰点后的拿铁清爽加倍。采用超高温瞬间灭菌工艺优质牛奶，保留众多营养物质</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/product/474/cafe_convert.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1519968030950.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰摩卡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>咖啡加上比利时进口可可粉，浓郁风味，口感柔滑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>温度降至冰点的摩卡咖啡，咖啡风味不减，口感柔滑令人爱不释手，清爽又不腻。选用比利时进口可可粉，可可脂含量26%，巧克力风味浓郁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/product/475/cafe_convert.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1519968041005.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰香草拿铁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最受女生喜爱的香草拿铁，难以抵抗的经典味道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>女生最爱的口味排名，香草一定在上位圈。清新淡雅的香荚兰风味，永不过时的经典风味，当然也要搭配精选阿拉比卡咖啡豆拼配的拿铁，口感更加丰富</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/product/1511168373722.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1519967174062.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰焦糖拿铁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>焦糖的存在，就是为了让苦涩的咖啡更加甜美可人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不习惯咖啡苦味的人，也难逃焦糖拿铁的魅力，忍不住为它疯狂打Call，爱上这枚小甜豆，感觉生活也会变甜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1526525783471.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1526526383947.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰榛果拿铁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>榛果的醇厚香甜，让味蕾有更深刻的美好记忆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>经典拿铁中加入优质榛果糖浆，冰块将甜度封存得刚刚好，加之榛果的醇香，带来丰富的满足感，让味蕾有更深刻的美好记忆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1526525453134.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1526526363021.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>热美式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>热拿铁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>热摩卡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰日晒耶加雪菲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高级别G1单品豆，日晒生豆处理，代号「浆果」</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>浆果——耶加雪菲高级别G1单品豆，日晒生豆处理，保留更多胶质，带来更加丰沛醇厚的味道。香气热烈似酒，香醇滑润的口感在众多豆子里别具一格。（容量12oz）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5b6277cb12d3ed723614ba0b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1531214294272.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1530067728048.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日晒耶加雪菲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高级别G1单品豆，日晒生豆处理，代号「浆果」</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>浆果——耶加雪菲高级别G1单品豆，日晒生豆处理，保留更多胶质，带来更加丰沛醇厚的味道。香气热烈似酒，香醇滑润的口感在众多豆子里别具一格。（容量12oz）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1531214311041.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1524128129311.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冻防弹咖啡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>防弹咖啡冰饮版本，低温下口感依然顺滑无比。咖啡因强势唤醒大脑，在黄油和椰子油的双重加持下为人体提供充足能量。一杯冻防弹，回到最佳状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>防弹咖啡冰饮版本，低碳无糖优脂，满足一天能量所需</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5b6277cb12d3ed723614ba0c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1529052424812.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1529052659283.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冻防弹路易波士</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>选用南非国宝茶路易波士制作而成，不含咖啡因</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>南非国宝茶路易波士搭配椰子油制作而成，优质脂肪与茶交融，爽滑醇香，路易波士自然的清甜带来多层次的丰富口感，不含咖啡因，满足不同时间需求</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1529052513013.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1529052703979.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>防弹咖啡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>低碳、无糖、优脂，完美的早餐从一杯防弹咖啡开始</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>咖啡因让大脑清醒，黄油和椰子油为人体提供所需能量。新西兰进口动物黄油，源自优质奶源，拥有香醇乳香味，冷榨椰子油中MCT含量高达60%以上</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1522815533303.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1519967221377.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>坚果防弹咖啡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>经典防弹咖啡中增添核桃香气，层次分明，风味独特</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>浓郁黄油基调上又增添了一味核桃的特殊香气，层次分明，风味独特，不含添加糖。（过敏源提示：本产品配料中含有坚果及其果仁制品）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1522815226805.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/product/1511084754388.jpeg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蔓莓无花果雪昔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无花果+黑糖+蔓越莓的惊喜组合，口感酸甜，不含咖啡因</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>融合了无花果果肉、古法黑糖与新鲜蔓越莓的多层次口感，自然的甜香\r\n中带有果肉的咀嚼感，蔓越莓中和了黑糖的甜，优质奶油混合清爽冰沙，不含咖啡因</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5b6277cb12d3ed723614ba0d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1531387856967.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1531388160806.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>摩卡奥利奥雪昔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>奥利奥饼干碎让咀嚼乐趣无处不在，经典不可替代</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>经典单品奥利奥饼干，现已加入摩卡雪昔人气饮品，带来非同一般的奇妙口感，巧克力风味浓郁，奥利奥饼干碎让咀嚼的乐趣无处不在，相信你会爱上它</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/product/1512354012382.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1519967150729.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>牛油果雪昔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>牛油果冰沙与淡奶油的“最佳拍档”，不含咖啡因</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰沙的清爽，奶油的醇香，互相平衡后的牛油果雪昔，天作之合的最佳搭配。不含咖啡因</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1526523674764.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/salegoods/1522301436271.jpg</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -77,7 +632,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -88,6 +643,33 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
@@ -111,16 +693,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -450,19 +1050,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="5" max="6" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="41.83203125" customWidth="1"/>
+    <col min="5" max="5" width="28.5" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
     <col min="7" max="7" width="26.1640625" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:10" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -484,33 +1089,1008 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1">
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="1">
+        <v>3300</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1">
+        <v>33</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2800</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1">
+        <v>28</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="1" customFormat="1">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2800</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="1">
+        <v>28</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3100</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="1">
+        <v>31</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3100</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="1">
+        <v>31</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2500</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="1">
+        <v>25</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2800</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="1">
+        <v>28</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2800</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="1">
+        <v>28</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2800</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="1">
+        <v>28</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="J10" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2800</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="1">
+        <v>28</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="1">
+        <v>3100</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="1">
+        <v>31</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J12" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2200</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="1">
+        <v>22</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J13" s="1">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2200</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="1">
+        <v>22</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J14" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2800</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="1">
+        <v>28</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="J15" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2800</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="1">
+        <v>28</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="J16" s="1">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" s="1">
+        <v>3100</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="1">
+        <v>31</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="J17" s="1">
         <v>11</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="1">
+        <v>3100</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="1">
+        <v>31</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="J18" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="1">
+        <v>3100</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" s="1">
+        <v>31</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="J19" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="1">
+        <v>3100</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F20" s="1">
+        <v>31</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="J20" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="1">
+        <v>3100</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F21" s="1">
+        <v>31</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="J21" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2800</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F22" s="1">
+        <v>28</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2800</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F23" s="1">
+        <v>28</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="1">
+        <v>3500</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F24" s="1">
+        <v>35</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="J24" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B25" s="1">
+        <v>3500</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F25" s="1">
+        <v>35</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="J25" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26" s="1">
+        <v>3500</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F26" s="1">
+        <v>35</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="J26" s="1">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B27" s="1">
+        <v>3500</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F27" s="1">
+        <v>35</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="J27" s="1">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B28" s="1">
+        <v>3500</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F28" s="1">
+        <v>35</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B29" s="1">
+        <v>3300</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F29" s="1">
+        <v>33</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="J29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B30" s="1">
+        <v>3500</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F30" s="1">
+        <v>35</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="J30" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="I2" r:id="rId2"/>
+    <hyperlink ref="H3" r:id="rId3"/>
+    <hyperlink ref="I3" r:id="rId4"/>
+    <hyperlink ref="H4" r:id="rId5"/>
+    <hyperlink ref="I4" r:id="rId6"/>
+    <hyperlink ref="H5" r:id="rId7"/>
+    <hyperlink ref="I5" r:id="rId8"/>
+    <hyperlink ref="H6" r:id="rId9"/>
+    <hyperlink ref="I6" r:id="rId10"/>
+    <hyperlink ref="H7" r:id="rId11"/>
+    <hyperlink ref="I7" r:id="rId12"/>
+    <hyperlink ref="H8" r:id="rId13"/>
+    <hyperlink ref="I8" r:id="rId14"/>
+    <hyperlink ref="H9" r:id="rId15"/>
+    <hyperlink ref="I9" r:id="rId16"/>
+    <hyperlink ref="H10" r:id="rId17"/>
+    <hyperlink ref="I10" r:id="rId18"/>
+    <hyperlink ref="H11" r:id="rId19"/>
+    <hyperlink ref="I11" r:id="rId20"/>
+    <hyperlink ref="H12" r:id="rId21"/>
+    <hyperlink ref="I12" r:id="rId22"/>
+    <hyperlink ref="H14" r:id="rId23"/>
+    <hyperlink ref="I14" r:id="rId24"/>
+    <hyperlink ref="H16" r:id="rId25"/>
+    <hyperlink ref="I16" r:id="rId26"/>
+    <hyperlink ref="H18" r:id="rId27"/>
+    <hyperlink ref="I18" r:id="rId28"/>
+    <hyperlink ref="H19" r:id="rId29"/>
+    <hyperlink ref="I19" r:id="rId30"/>
+    <hyperlink ref="H20" r:id="rId31"/>
+    <hyperlink ref="I20" r:id="rId32"/>
+    <hyperlink ref="H21" r:id="rId33"/>
+    <hyperlink ref="I21" r:id="rId34"/>
+    <hyperlink ref="H13" r:id="rId35"/>
+    <hyperlink ref="I13" r:id="rId36"/>
+    <hyperlink ref="H15" r:id="rId37"/>
+    <hyperlink ref="I15" r:id="rId38"/>
+    <hyperlink ref="H17" r:id="rId39"/>
+    <hyperlink ref="I17" r:id="rId40"/>
+    <hyperlink ref="H22" r:id="rId41"/>
+    <hyperlink ref="I22" r:id="rId42"/>
+    <hyperlink ref="H23" r:id="rId43"/>
+    <hyperlink ref="I23" r:id="rId44"/>
+    <hyperlink ref="H24" r:id="rId45"/>
+    <hyperlink ref="I24" r:id="rId46"/>
+    <hyperlink ref="H25" r:id="rId47"/>
+    <hyperlink ref="I25" r:id="rId48"/>
+    <hyperlink ref="H26" r:id="rId49"/>
+    <hyperlink ref="I26" r:id="rId50"/>
+    <hyperlink ref="H27" r:id="rId51"/>
+    <hyperlink ref="I27" r:id="rId52"/>
+    <hyperlink ref="H28" r:id="rId53"/>
+    <hyperlink ref="I28" r:id="rId54"/>
+    <hyperlink ref="H29" r:id="rId55"/>
+    <hyperlink ref="I29" r:id="rId56"/>
+    <hyperlink ref="H30" r:id="rId57"/>
+    <hyperlink ref="I30" r:id="rId58"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
add group activity fake data
</commit_message>
<xml_diff>
--- a/src/utils/coffee.xlsx
+++ b/src/utils/coffee.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="coffee" sheetId="1" r:id="rId1"/>
     <sheet name="coffee-category" sheetId="2" r:id="rId2"/>
+    <sheet name="group-rule" sheetId="3" r:id="rId3"/>
+    <sheet name="group-activity" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="219">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -770,6 +772,141 @@
   </si>
   <si>
     <t>https://images.lyancafe.com/menucategory/1531471349491.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>title</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>textImageUrl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shareDataDto</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ruleText</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>explainText</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有折</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/provider/1529045466914.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拼团活动规则</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1、拼团活动共分两种：老带新团+全民参与，购买万能咖啡请点击全民参与进入。*注：老带新团，入库后单杯配送需另付5元，两杯及以上可免配送费。\r\n*2、老带新团，老用户仅可开团，新用户可直接参团或开团。（注：新用户指未购买过任何Coffee Box产品的用户）新用户仅可享受一次直接参与新人福利团的机会。若该次拼团失败，可重新参与其他拼团。拼团成功后可发起其他拼团。\r\n\r\n*3、全民参与团，新老用户皆可参团或开团。\r\n*4、拼团成功，饮品将直接存入咖啡库。请至“个人中心-我的咖啡库”下单饮用或按流程提示操作。\r\n*5、拼团失败，金额将原路返还。如有其他疑问可直接联系连咖啡线上客服。\r\n*6、关于拼团活动截止时间，限时限量拼团售完即止。\r\n*7、具体配送服务范围：*上海：黄浦区，静安区，虹口区，徐汇区，长宁区，五角场，漕河泾开发区，陆家嘴，塘桥，浦东大道，上海科技馆，金桥，张江；*北京：中关村，西单，金融街，宣武门，望京，三元桥，亮马桥，三里屯，朝阳门，团结湖，呼家楼，四惠，八里庄，双井，劲松，西二旗，上地， 酒仙桥（将台）、东直门、国贸、惠新西街、北太平庄、新街口、和平里、花园桥、紫竹桥、崇文门、大望路、安贞；*广州：中心城区，海珠区，荔湾区，越秀区，天河区，白云区部分区域；*深圳：南山区：科技园、深圳大学、软件产业基地、滨海之窗、海岸城、桃园、前海、蛇口网谷、海上世界、招商局、蛇口医院、南山医院 ；福田区： 车公庙、竹子林、泰然工业区 、会展中心、市民广场、岗厦、皇岗、福田区政府、福田CBD、香蜜湖 、华强北、华强南、科学馆 ；保税区：全境服务 ；罗湖区:老街、国贸 、东门美食街、京基100 、金光华。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+        "appId": null,
+        "imgUrl": "https://qaimages.lyancafe.com/giftPacks/1509628466128.png",
+        "link": "/vip/index",
+        "desc": "可与其他优惠叠加",
+        "title": "连咖啡尊享会员限时开放，折上再享8.8折",
+        "timeLineTitle": "连咖啡尊享会员限时开放，折上再享8.8折",
+        "orderId": 0,
+        "giftCafeTraceId": 0,
+        "orderType": 0,
+        "freeOrder": false
+      }</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>oldPrice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>finalPrice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>groupAccountLabel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>priceLabel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>imageUrl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sort</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>timeLeft</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>inventoryLeft</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>限时专享 | 热太妃榛果拿铁 1杯装</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/groupActivity/1531703858228.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>限时专享 | 冰榛果拿铁 1杯装</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/groupActivity/1526969234769.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>限时闪购 | 牛油果雪昔 1杯装</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/groupActivity/1529547446495.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抢先品鉴 | 冰焦糖拿铁 1杯装</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/groupActivity/1528251741779.jpeg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1元1杯 | 冰美式 1杯装</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://images.lyancafe.com/groupActivity/1524897134622.png</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -845,7 +982,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -859,6 +996,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2248,7 +2388,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -2480,4 +2620,306 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="58.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
+    <col min="5" max="5" width="39" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="285">
+      <c r="A2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="47" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61" customWidth="1"/>
+    <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>33</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>581121453</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>31</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="J3">
+        <v>5</v>
+      </c>
+      <c r="K3">
+        <v>-196478546</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>35</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="J4">
+        <v>9</v>
+      </c>
+      <c r="K4">
+        <v>1185921455</v>
+      </c>
+      <c r="L4">
+        <v>48093</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>31</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>1149921456</v>
+      </c>
+      <c r="L5">
+        <v>879719</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>217</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>22</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="J6">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink ref="I5" r:id="rId4"/>
+    <hyperlink ref="I6" r:id="rId5"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>